<commit_message>
Update Cuadro A1 - Población total por sexo, grupos quinquenales de edad y área.xlsx
</commit_message>
<xml_diff>
--- a/Guatemala/CENSO 2018/Cuadro A1 - Población total por sexo, grupos quinquenales de edad y área.xlsx
+++ b/Guatemala/CENSO 2018/Cuadro A1 - Población total por sexo, grupos quinquenales de edad y área.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-MUNI\Guatemala\CENSO 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D610CC92-1202-47EE-A787-93D04EBAE5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3273BDC2-5DD4-449C-ADC2-86B543AC4B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A1_1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="408">
   <si>
     <t>Características generales de la población. Censo 2018</t>
   </si>
@@ -1275,7 +1275,7 @@
     <numFmt numFmtId="164" formatCode="##\ ###\ ###\ ###\ ##0"/>
     <numFmt numFmtId="165" formatCode=".\ \ \ \ ##0;000000000000000000000000000000000000000000000000000000000000000000000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1346,6 +1346,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1441,7 +1448,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1532,21 +1539,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1556,7 +1549,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1565,6 +1575,42 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="36">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2734,42 +2780,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2784,45 +2794,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{546BF888-D580-4725-885E-A188B7B4DE5C}" name="Población" displayName="Población" ref="A5:AF346" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" headerRowCellStyle="Neutral">
-  <autoFilter ref="A5:AF346" xr:uid="{D55912E5-1C26-43B0-946A-8B7E12ABC44F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{546BF888-D580-4725-885E-A188B7B4DE5C}" name="Población" displayName="Población" ref="A5:AF345" totalsRowShown="0" headerRowDxfId="0" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" headerRowCellStyle="Neutral">
+  <autoFilter ref="A5:AF345" xr:uid="{D55912E5-1C26-43B0-946A-8B7E12ABC44F}"/>
   <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{DB55B1E0-A2B5-4316-A586-9DD10EEC3F35}" name="Código" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{D1FA5CAD-96F6-4092-BC59-1ED5003A6D0B}" name="Departamento" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{D777CC2F-288A-4FE5-8C2C-A1B3DFEEC461}" name="Código2" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{C3CFAA88-C320-4FA7-B344-FCB29882EAC4}" name="Municipio" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{FC39CA06-A055-4C3C-AA36-B131CF11A2E7}" name="Población total" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{5149E000-011C-4882-80D6-7A748FFB914F}" name="Hombres" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{E4728424-5B5D-4E25-8C46-66813CEFFE84}" name="Mujeres" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{E95DB9E1-0743-4B9A-A1BC-8C798E74547D}" name="Mujeres (%)" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{DB55B1E0-A2B5-4316-A586-9DD10EEC3F35}" name="Código" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{D1FA5CAD-96F6-4092-BC59-1ED5003A6D0B}" name="Departamento" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{D777CC2F-288A-4FE5-8C2C-A1B3DFEEC461}" name="Código2" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{C3CFAA88-C320-4FA7-B344-FCB29882EAC4}" name="Municipio" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{FC39CA06-A055-4C3C-AA36-B131CF11A2E7}" name="Población total" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{5149E000-011C-4882-80D6-7A748FFB914F}" name="Hombres" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{E4728424-5B5D-4E25-8C46-66813CEFFE84}" name="Mujeres" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{E95DB9E1-0743-4B9A-A1BC-8C798E74547D}" name="Mujeres (%)" dataDxfId="25">
       <calculatedColumnFormula>+G6/E6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{86FD656C-558A-4685-9839-47786D326705}" name="Hombres (%)" dataDxfId="23">
+    <tableColumn id="9" xr3:uid="{86FD656C-558A-4685-9839-47786D326705}" name="Hombres (%)" dataDxfId="24">
       <calculatedColumnFormula>+F6/E6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A24039F6-0B63-49D8-812B-B25BC91DCBFC}" name="Población Urbana" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{C0280005-2A6A-4B45-A58A-403557F9CF19}" name="Población Rural" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{7AD343E0-720E-42BC-8AC3-3E4517CBC210}" name="0 - 4" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{5D6712F7-339F-42D4-B507-E4D6D77191EF}" name="5 - 9" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{220E970C-F5F8-4F05-8F6A-9B343E1ADEB9}" name="10 - 14" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{EC871ABA-95EA-4115-B6E1-EF5E3E02D692}" name="15 - 19" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{3718FBF9-6C9D-4158-8B81-6B9575897893}" name="20 - 24" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{601BF7D3-51AC-4642-8BEF-55E039D34AC4}" name="25 - 29" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{F6A78843-F959-45DC-945D-F70AD769B4A5}" name="30 - 34" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{9BC807B2-56CD-4B83-A887-284A05509898}" name="35 - 39" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{78047AC1-083A-46D8-8CFA-B7A9D438AE8B}" name="40 - 44" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{D1562DAE-5A21-4A6C-A4F1-90EA4AA53980}" name="45 - 49" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{8BEB8C07-4031-4165-8DA3-0C2FB8935D92}" name="50 - 54" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{787E8BD7-7078-49EA-9F5F-E0B9E30254ED}" name="55 - 59" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{64C389BE-EB12-4041-B7D5-76CB08038ADB}" name="60 - 64" dataDxfId="8"/>
-    <tableColumn id="25" xr3:uid="{7D9355F4-A596-466B-A694-7A75DCE8D058}" name="65 - 69" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{B16FC9DC-8DA8-4427-9B9B-6D303002260E}" name="70  - 74" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{04E241A5-DCE6-4668-8621-4259A10CA17C}" name="75 - 79" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{B4D1E386-BA04-4D7B-8595-5F810562810D}" name="80 - 84" dataDxfId="4"/>
-    <tableColumn id="29" xr3:uid="{5E379281-EA41-4923-A933-0D7BAA3E0658}" name="85 - 89" dataDxfId="3"/>
-    <tableColumn id="30" xr3:uid="{87C29544-601A-4264-B7DA-649281A9F8C6}" name="90  - 94" dataDxfId="2"/>
-    <tableColumn id="31" xr3:uid="{0D140DB5-4DEB-482E-AD30-26E2AB86C0C9}" name="95 - 99" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{B246ADB6-24B4-4CD3-AA15-35A00ED6F3E1}" name="100 o más" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{A24039F6-0B63-49D8-812B-B25BC91DCBFC}" name="Población Urbana" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{C0280005-2A6A-4B45-A58A-403557F9CF19}" name="Población Rural" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{7AD343E0-720E-42BC-8AC3-3E4517CBC210}" name="0 - 4" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{5D6712F7-339F-42D4-B507-E4D6D77191EF}" name="5 - 9" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{220E970C-F5F8-4F05-8F6A-9B343E1ADEB9}" name="10 - 14" dataDxfId="19"/>
+    <tableColumn id="15" xr3:uid="{EC871ABA-95EA-4115-B6E1-EF5E3E02D692}" name="15 - 19" dataDxfId="18"/>
+    <tableColumn id="16" xr3:uid="{3718FBF9-6C9D-4158-8B81-6B9575897893}" name="20 - 24" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{601BF7D3-51AC-4642-8BEF-55E039D34AC4}" name="25 - 29" dataDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{F6A78843-F959-45DC-945D-F70AD769B4A5}" name="30 - 34" dataDxfId="15"/>
+    <tableColumn id="19" xr3:uid="{9BC807B2-56CD-4B83-A887-284A05509898}" name="35 - 39" dataDxfId="14"/>
+    <tableColumn id="20" xr3:uid="{78047AC1-083A-46D8-8CFA-B7A9D438AE8B}" name="40 - 44" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{D1562DAE-5A21-4A6C-A4F1-90EA4AA53980}" name="45 - 49" dataDxfId="12"/>
+    <tableColumn id="22" xr3:uid="{8BEB8C07-4031-4165-8DA3-0C2FB8935D92}" name="50 - 54" dataDxfId="11"/>
+    <tableColumn id="23" xr3:uid="{787E8BD7-7078-49EA-9F5F-E0B9E30254ED}" name="55 - 59" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{64C389BE-EB12-4041-B7D5-76CB08038ADB}" name="60 - 64" dataDxfId="9"/>
+    <tableColumn id="25" xr3:uid="{7D9355F4-A596-466B-A694-7A75DCE8D058}" name="65 - 69" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{B16FC9DC-8DA8-4427-9B9B-6D303002260E}" name="70  - 74" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{04E241A5-DCE6-4668-8621-4259A10CA17C}" name="75 - 79" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{B4D1E386-BA04-4D7B-8595-5F810562810D}" name="80 - 84" dataDxfId="5"/>
+    <tableColumn id="29" xr3:uid="{5E379281-EA41-4923-A933-0D7BAA3E0658}" name="85 - 89" dataDxfId="4"/>
+    <tableColumn id="30" xr3:uid="{87C29544-601A-4264-B7DA-649281A9F8C6}" name="90  - 94" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{0D140DB5-4DEB-482E-AD30-26E2AB86C0C9}" name="95 - 99" dataDxfId="2"/>
+    <tableColumn id="32" xr3:uid="{B246ADB6-24B4-4CD3-AA15-35A00ED6F3E1}" name="100 o más" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3107,7 +3117,9 @@
   </sheetPr>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:Z31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3136,51 +3148,51 @@
       </c>
     </row>
     <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="45" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45" t="s">
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="45"/>
+      <c r="AB5" s="41"/>
     </row>
     <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
@@ -5344,10 +5356,10 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AH346"/>
+  <dimension ref="A1:AF345"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:AF5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:AF345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5389,101 +5401,101 @@
       </c>
       <c r="C2" s="28"/>
     </row>
-    <row r="5" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+    <row r="5" spans="1:32" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="44" t="s">
         <v>384</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="46" t="s">
         <v>380</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="47" t="s">
         <v>382</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="47" t="s">
         <v>383</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="44" t="s">
+      <c r="M5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="44" t="s">
+      <c r="N5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="44" t="s">
+      <c r="P5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="44" t="s">
+      <c r="Q5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="44" t="s">
+      <c r="R5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="44" t="s">
+      <c r="S5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="44" t="s">
+      <c r="T5" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="44" t="s">
+      <c r="V5" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="44" t="s">
+      <c r="W5" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="44" t="s">
+      <c r="X5" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="Y5" s="44" t="s">
+      <c r="Y5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="Z5" s="44" t="s">
+      <c r="Z5" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="AA5" s="44" t="s">
+      <c r="AA5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="AB5" s="44" t="s">
+      <c r="AB5" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="AC5" s="44" t="s">
+      <c r="AC5" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="AD5" s="44" t="s">
+      <c r="AD5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AE5" s="44" t="s">
+      <c r="AE5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="AF5" s="44" t="s">
+      <c r="AF5" s="48" t="s">
         <v>30</v>
       </c>
     </row>
@@ -37610,11 +37622,11 @@
         <v>14311</v>
       </c>
       <c r="H327" s="39">
-        <f t="shared" ref="H327:H346" si="10">+G327/E327</f>
+        <f t="shared" ref="H327:H345" si="10">+G327/E327</f>
         <v>0.52317759742633618</v>
       </c>
       <c r="I327" s="39">
-        <f t="shared" ref="I327:I346" si="11">+F327/E327</f>
+        <f t="shared" ref="I327:I345" si="11">+F327/E327</f>
         <v>0.47682240257366382</v>
       </c>
       <c r="J327" s="31">
@@ -38587,7 +38599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A337" s="10">
         <v>22</v>
       </c>
@@ -38687,7 +38699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A338" s="10">
         <v>22</v>
       </c>
@@ -38787,7 +38799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A339" s="10">
         <v>22</v>
       </c>
@@ -38887,7 +38899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A340" s="10">
         <v>22</v>
       </c>
@@ -38987,7 +38999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A341" s="10">
         <v>22</v>
       </c>
@@ -39087,7 +39099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="342" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A342" s="10">
         <v>22</v>
       </c>
@@ -39187,7 +39199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A343" s="10">
         <v>22</v>
       </c>
@@ -39287,7 +39299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A344" s="10">
         <v>22</v>
       </c>
@@ -39387,7 +39399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A345" s="21">
         <v>22</v>
       </c>
@@ -39486,49 +39498,6 @@
       <c r="AF345" s="38">
         <v>2</v>
       </c>
-    </row>
-    <row r="346" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A346" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B346" s="11"/>
-      <c r="D346" s="30"/>
-      <c r="E346" s="26"/>
-      <c r="F346" s="26"/>
-      <c r="G346" s="26"/>
-      <c r="H346" s="39" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I346" s="39" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J346" s="39"/>
-      <c r="K346" s="39"/>
-      <c r="L346" s="26"/>
-      <c r="M346" s="26"/>
-      <c r="N346" s="26"/>
-      <c r="O346" s="26"/>
-      <c r="P346" s="26"/>
-      <c r="Q346" s="26"/>
-      <c r="R346" s="26"/>
-      <c r="S346" s="26"/>
-      <c r="T346" s="26"/>
-      <c r="U346" s="26"/>
-      <c r="V346" s="26"/>
-      <c r="W346" s="26"/>
-      <c r="X346" s="26"/>
-      <c r="Y346" s="26"/>
-      <c r="Z346" s="26"/>
-      <c r="AA346" s="26"/>
-      <c r="AB346" s="26"/>
-      <c r="AC346" s="26"/>
-      <c r="AD346" s="26"/>
-      <c r="AE346" s="26"/>
-      <c r="AF346" s="26"/>
-      <c r="AG346" s="26"/>
-      <c r="AH346" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -39548,7 +39517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFD5627-C7B7-41CB-B8FF-ED3219DDB42A}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -39567,7 +39536,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="40" t="s">
         <v>385</v>
       </c>
       <c r="B2" t="s">
@@ -39575,7 +39544,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="40" t="s">
         <v>386</v>
       </c>
       <c r="B3" t="s">
@@ -39583,7 +39552,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="40" t="s">
         <v>387</v>
       </c>
       <c r="B4" t="s">
@@ -39591,7 +39560,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="40" t="s">
         <v>388</v>
       </c>
       <c r="B5" t="s">
@@ -39599,7 +39568,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="40" t="s">
         <v>389</v>
       </c>
       <c r="B6" t="s">
@@ -39607,7 +39576,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="40" t="s">
         <v>390</v>
       </c>
       <c r="B7" t="s">
@@ -39615,7 +39584,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="40" t="s">
         <v>391</v>
       </c>
       <c r="B8" t="s">
@@ -39623,7 +39592,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="40" t="s">
         <v>392</v>
       </c>
       <c r="B9" t="s">
@@ -39631,7 +39600,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="40" t="s">
         <v>393</v>
       </c>
       <c r="B10" t="s">
@@ -39639,7 +39608,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="40" t="s">
         <v>394</v>
       </c>
       <c r="B11" t="s">
@@ -39647,7 +39616,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="40" t="s">
         <v>395</v>
       </c>
       <c r="B12" t="s">
@@ -39655,7 +39624,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="40" t="s">
         <v>396</v>
       </c>
       <c r="B13" t="s">
@@ -39663,7 +39632,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="40" t="s">
         <v>397</v>
       </c>
       <c r="B14" t="s">
@@ -39671,7 +39640,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="40" t="s">
         <v>398</v>
       </c>
       <c r="B15" t="s">
@@ -39679,7 +39648,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="40" t="s">
         <v>399</v>
       </c>
       <c r="B16" t="s">
@@ -39687,7 +39656,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="40" t="s">
         <v>400</v>
       </c>
       <c r="B17" t="s">
@@ -39695,7 +39664,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="40" t="s">
         <v>401</v>
       </c>
       <c r="B18" t="s">
@@ -39703,7 +39672,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="40" t="s">
         <v>402</v>
       </c>
       <c r="B19" t="s">
@@ -39711,7 +39680,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="40" t="s">
         <v>403</v>
       </c>
       <c r="B20" t="s">
@@ -39719,7 +39688,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="40" t="s">
         <v>404</v>
       </c>
       <c r="B21" t="s">
@@ -39727,7 +39696,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="40" t="s">
         <v>405</v>
       </c>
       <c r="B22" t="s">
@@ -39748,7 +39717,7 @@
   <dimension ref="B4:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B24"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>